<commit_message>
Started to look at LA (Local Area) database.
</commit_message>
<xml_diff>
--- a/Metro Divisions.xlsx
+++ b/Metro Divisions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris.kiniry\Documents\R Projects\BLS\"/>
@@ -309,7 +309,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +319,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,9 +341,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B61"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B61" sqref="B3:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +672,7 @@
     <col min="2" max="2" width="77.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,15 +680,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16980</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -688,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -696,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -704,7 +715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -712,15 +723,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -728,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -736,15 +750,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>19820</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -752,7 +769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -760,15 +777,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>31080</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -776,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -784,15 +804,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>33100</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -800,7 +823,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -808,7 +831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -816,15 +839,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>35620</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -832,7 +858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -840,7 +866,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -848,7 +874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -856,15 +882,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>37980</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -872,7 +901,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -880,7 +909,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -888,7 +917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -896,15 +925,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>41860</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -912,7 +944,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -920,7 +952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -928,15 +960,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42660</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -944,7 +979,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>62</v>
       </c>
@@ -952,15 +987,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47900</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>65</v>
       </c>
@@ -968,7 +1006,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -976,15 +1014,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>71650</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -992,7 +1033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -1000,7 +1041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -1008,7 +1049,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -1016,7 +1057,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>78</v>
       </c>
@@ -1024,7 +1065,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -1032,7 +1073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -1040,7 +1081,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -1048,15 +1089,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>86</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>88</v>
       </c>

</xml_diff>